<commit_message>
Changes for Portfolio 31072022
Small changes to increase portfolio experience
</commit_message>
<xml_diff>
--- a/4. Project - Python/05 Sent to Client/Final_report.xlsx
+++ b/4. Project - Python/05 Sent to Client/Final_report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Data_Analytic\JUPYTER\Second\05 Sent to Client\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35476006-9860-4D21-9E10-A6A2C1802787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C40EA17-F17E-45BB-97FB-4F1FF554F3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="808" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="808" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Title Page" sheetId="1" r:id="rId1"/>
@@ -17085,256 +17085,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>333</xdr:row>
-      <xdr:rowOff>138546</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>310186</xdr:colOff>
-      <xdr:row>350</xdr:row>
-      <xdr:rowOff>36554</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="76" name="Picture 75">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53363D74-54AF-9D11-068B-C91B3F64341D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6338455" y="67004046"/>
-          <a:ext cx="3098413" cy="3136508"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>582954</xdr:colOff>
-      <xdr:row>351</xdr:row>
-      <xdr:rowOff>28773</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>351631</xdr:colOff>
-      <xdr:row>367</xdr:row>
-      <xdr:rowOff>117281</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="79" name="Picture 78">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F48D98C-0C92-138C-9F78-3B227040A70F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3197999" y="70323273"/>
-          <a:ext cx="3301587" cy="3136508"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>40226</xdr:colOff>
-      <xdr:row>334</xdr:row>
-      <xdr:rowOff>144136</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>12079</xdr:colOff>
-      <xdr:row>351</xdr:row>
-      <xdr:rowOff>42144</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="82" name="Picture 81">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9445213F-015A-58C8-FA82-FBFF311ED374}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12110999" y="67200136"/>
-          <a:ext cx="3504762" cy="3136508"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>120954</xdr:colOff>
-      <xdr:row>333</xdr:row>
-      <xdr:rowOff>51682</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>3918</xdr:colOff>
-      <xdr:row>349</xdr:row>
-      <xdr:rowOff>140190</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="85" name="Picture 84">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64A90675-38F4-6420-EC40-689B0A4886BE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="969545" y="66917182"/>
-          <a:ext cx="3415873" cy="3136508"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>426818</xdr:colOff>
-      <xdr:row>351</xdr:row>
-      <xdr:rowOff>45818</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>416060</xdr:colOff>
-      <xdr:row>367</xdr:row>
-      <xdr:rowOff>134326</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="87" name="Picture 86">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BCBBC54-ECFE-1D1D-646D-6CD87393BAEB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9553500" y="70340318"/>
-          <a:ext cx="2933333" cy="3136508"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>299726</xdr:colOff>
       <xdr:row>311</xdr:row>
@@ -17360,7 +17110,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -17375,356 +17125,6 @@
         <a:xfrm>
           <a:off x="559499" y="62818364"/>
           <a:ext cx="5358730" cy="3834920"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>368</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>148255</xdr:colOff>
-      <xdr:row>385</xdr:row>
-      <xdr:rowOff>177373</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="91" name="Picture 90">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{078F753D-84CE-0DBC-3540-98204E222C21}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1437409" y="74831864"/>
-          <a:ext cx="5447619" cy="3415873"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>346363</xdr:colOff>
-      <xdr:row>390</xdr:row>
-      <xdr:rowOff>173182</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>486611</xdr:colOff>
-      <xdr:row>407</xdr:row>
-      <xdr:rowOff>71190</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="93" name="Picture 92">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{921E3BFB-2D94-1689-7C8D-ED69F1F14AF4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="606136" y="80217818"/>
-          <a:ext cx="4850793" cy="3136508"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>98044</xdr:colOff>
-      <xdr:row>391</xdr:row>
-      <xdr:rowOff>46092</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>281079</xdr:colOff>
-      <xdr:row>407</xdr:row>
-      <xdr:rowOff>134600</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="95" name="Picture 94">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7EA41CF-AEDB-9043-91AE-C2D48BD68A92}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11579999" y="80281228"/>
-          <a:ext cx="4304762" cy="3136508"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>40226</xdr:colOff>
-      <xdr:row>391</xdr:row>
-      <xdr:rowOff>5592</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>6156</xdr:colOff>
-      <xdr:row>407</xdr:row>
-      <xdr:rowOff>94100</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="97" name="Picture 96">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F2275E1-1EB8-8F07-993F-F5243920719A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6188181" y="80240728"/>
-          <a:ext cx="4711111" cy="3136508"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>190227</xdr:colOff>
-      <xdr:row>410</xdr:row>
-      <xdr:rowOff>103636</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>317777</xdr:colOff>
-      <xdr:row>427</xdr:row>
-      <xdr:rowOff>1644</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="99" name="Picture 98">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{967B1EC8-64D3-9F69-5A81-835ACAF091B6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="450000" y="83958272"/>
-          <a:ext cx="4838095" cy="3136508"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>218999</xdr:colOff>
-      <xdr:row>411</xdr:row>
-      <xdr:rowOff>149728</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>418191</xdr:colOff>
-      <xdr:row>428</xdr:row>
-      <xdr:rowOff>47736</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="101" name="Picture 100">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07BDB647-CD26-9FB5-80DF-7DDE5A5CD23E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6366954" y="84194864"/>
-          <a:ext cx="4355555" cy="3136508"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>386317</xdr:colOff>
-      <xdr:row>412</xdr:row>
-      <xdr:rowOff>57273</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>391574</xdr:colOff>
-      <xdr:row>428</xdr:row>
-      <xdr:rowOff>145781</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="103" name="Picture 102">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D075C7A9-38DD-2109-FF69-2A3D8AAB1B6C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11868272" y="84292909"/>
-          <a:ext cx="4126984" cy="3136508"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17760,7 +17160,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -17810,7 +17210,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -17860,7 +17260,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -17875,6 +17275,656 @@
         <a:xfrm>
           <a:off x="6517226" y="92761774"/>
           <a:ext cx="7772400" cy="4468143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>517071</xdr:colOff>
+      <xdr:row>367</xdr:row>
+      <xdr:rowOff>1374322</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>108856</xdr:colOff>
+      <xdr:row>387</xdr:row>
+      <xdr:rowOff>79169</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53DC33CE-89FC-3F42-55DC-E193FC2CEED5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="789214" y="74716822"/>
+          <a:ext cx="6613071" cy="3807526"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>324644</xdr:colOff>
+      <xdr:row>352</xdr:row>
+      <xdr:rowOff>94535</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>579364</xdr:colOff>
+      <xdr:row>367</xdr:row>
+      <xdr:rowOff>373543</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="Picture 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DD9F78E-444C-425D-82A0-5146844BC4E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5862751" y="70579535"/>
+          <a:ext cx="3221077" cy="3136508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>38079</xdr:colOff>
+      <xdr:row>332</xdr:row>
+      <xdr:rowOff>182684</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>569682</xdr:colOff>
+      <xdr:row>351</xdr:row>
+      <xdr:rowOff>80692</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Picture 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A77A9AC2-8E15-4673-A01D-03F1A06DCBD6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10297865" y="66857684"/>
+          <a:ext cx="3457138" cy="3517508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>313133</xdr:colOff>
+      <xdr:row>352</xdr:row>
+      <xdr:rowOff>29936</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>281245</xdr:colOff>
+      <xdr:row>367</xdr:row>
+      <xdr:rowOff>308944</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="Picture 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2136841-AAB0-4DD7-8ED4-E756DC86E027}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10572919" y="70514936"/>
+          <a:ext cx="2893647" cy="3136508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>102053</xdr:colOff>
+      <xdr:row>351</xdr:row>
+      <xdr:rowOff>169447</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>72971</xdr:colOff>
+      <xdr:row>367</xdr:row>
+      <xdr:rowOff>257955</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Picture 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20C7A33A-7356-489F-B0EC-C22C82DC3B94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="959303" y="70463947"/>
+          <a:ext cx="4066668" cy="3136508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>297750</xdr:colOff>
+      <xdr:row>408</xdr:row>
+      <xdr:rowOff>101640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>371823</xdr:colOff>
+      <xdr:row>424</xdr:row>
+      <xdr:rowOff>190148</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="46" name="Picture 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1C02378-2211-452A-9709-C2824EEF4502}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6420964" y="83567854"/>
+          <a:ext cx="4210645" cy="3136508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>447440</xdr:colOff>
+      <xdr:row>390</xdr:row>
+      <xdr:rowOff>88353</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>414194</xdr:colOff>
+      <xdr:row>406</xdr:row>
+      <xdr:rowOff>176861</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="Picture 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{210ED133-8C1C-48BA-BFBF-4D10F9F9721B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11292333" y="80125567"/>
+          <a:ext cx="4647611" cy="3136508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>201621</xdr:colOff>
+      <xdr:row>408</xdr:row>
+      <xdr:rowOff>140034</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>177293</xdr:colOff>
+      <xdr:row>425</xdr:row>
+      <xdr:rowOff>38042</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="49" name="Picture 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7174F22A-74E3-45C7-9EC2-244870D4F96D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11631621" y="83606248"/>
+          <a:ext cx="4071422" cy="3136508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>455195</xdr:colOff>
+      <xdr:row>390</xdr:row>
+      <xdr:rowOff>11340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>561630</xdr:colOff>
+      <xdr:row>406</xdr:row>
+      <xdr:rowOff>99848</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="50" name="Picture 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFC89522-5DE3-4793-91C4-486700627FB7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5993302" y="80048554"/>
+          <a:ext cx="4828114" cy="3136508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>572143</xdr:colOff>
+      <xdr:row>390</xdr:row>
+      <xdr:rowOff>12626</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>262716</xdr:colOff>
+      <xdr:row>406</xdr:row>
+      <xdr:rowOff>101134</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="53" name="Picture 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35DC8D8E-4796-4907-9C4A-57A8049C8C04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="844286" y="80049840"/>
+          <a:ext cx="4371430" cy="3136508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>149678</xdr:colOff>
+      <xdr:row>332</xdr:row>
+      <xdr:rowOff>122465</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>54908</xdr:colOff>
+      <xdr:row>349</xdr:row>
+      <xdr:rowOff>20473</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="55" name="Picture 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBC1F1D2-6387-4DCF-BE79-467C7A6CB465}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1006928" y="66797465"/>
+          <a:ext cx="3415873" cy="3136508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>405946</xdr:colOff>
+      <xdr:row>333</xdr:row>
+      <xdr:rowOff>106590</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>538002</xdr:colOff>
+      <xdr:row>350</xdr:row>
+      <xdr:rowOff>4598</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="56" name="Picture 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15F5E4CF-7F20-464C-824F-B279BB233FE2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5944053" y="66972090"/>
+          <a:ext cx="3098413" cy="3136508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>409</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>157238</xdr:colOff>
+      <xdr:row>425</xdr:row>
+      <xdr:rowOff>88508</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="57" name="Picture 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABF25E5D-28F5-4911-B562-C204D81F66CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="857250" y="83656714"/>
+          <a:ext cx="4838095" cy="3136508"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -19942,256 +19992,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>421143</xdr:colOff>
-      <xdr:row>514</xdr:row>
-      <xdr:rowOff>185182</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>542994</xdr:colOff>
-      <xdr:row>531</xdr:row>
-      <xdr:rowOff>83190</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="127" name="Picture 126">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7A7BD90-50BD-4072-9958-F85EDB3D9CB3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6636206" y="101531182"/>
-          <a:ext cx="3098413" cy="3136508"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>257250</xdr:colOff>
-      <xdr:row>532</xdr:row>
-      <xdr:rowOff>75409</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>582274</xdr:colOff>
-      <xdr:row>548</xdr:row>
-      <xdr:rowOff>163917</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="128" name="Picture 127">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{729C9947-56E5-4752-9CE4-1DDC523F153D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3495750" y="104850409"/>
-          <a:ext cx="3301587" cy="3136508"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>240562</xdr:colOff>
-      <xdr:row>516</xdr:row>
-      <xdr:rowOff>272</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>173449</xdr:colOff>
-      <xdr:row>532</xdr:row>
-      <xdr:rowOff>88780</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="129" name="Picture 128">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09EA790F-D63D-423C-9623-031A460B081A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12408750" y="101727272"/>
-          <a:ext cx="3504762" cy="3136508"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>410046</xdr:colOff>
-      <xdr:row>514</xdr:row>
-      <xdr:rowOff>98318</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>254044</xdr:colOff>
-      <xdr:row>530</xdr:row>
-      <xdr:rowOff>186826</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="130" name="Picture 129">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC62612F-F3C2-478F-BFDF-D1B062CA2E3F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1267296" y="101444318"/>
-          <a:ext cx="3415873" cy="3136508"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>64313</xdr:colOff>
-      <xdr:row>532</xdr:row>
-      <xdr:rowOff>92454</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>21084</xdr:colOff>
-      <xdr:row>548</xdr:row>
-      <xdr:rowOff>180962</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="131" name="Picture 130">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0FDF8C4-A832-44BA-A79E-B0453624B281}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9851251" y="104867454"/>
-          <a:ext cx="2933333" cy="3136508"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>493</xdr:row>
@@ -20217,7 +20017,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -20232,356 +20032,6 @@
         <a:xfrm>
           <a:off x="857250" y="97345500"/>
           <a:ext cx="5358730" cy="3834920"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>71437</xdr:colOff>
-      <xdr:row>555</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>161243</xdr:colOff>
-      <xdr:row>573</xdr:row>
-      <xdr:rowOff>34498</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="133" name="Picture 132">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C64F8222-9FC4-4261-9658-6291B88FF4BA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="928687" y="109204125"/>
-          <a:ext cx="5447619" cy="3415873"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>156136</xdr:colOff>
-      <xdr:row>578</xdr:row>
-      <xdr:rowOff>190496</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>244429</xdr:colOff>
-      <xdr:row>595</xdr:row>
-      <xdr:rowOff>88504</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="134" name="Picture 133">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CC22F01-9B24-4758-8865-9B4575F1655A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1013386" y="113728496"/>
-          <a:ext cx="4850793" cy="3136508"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>414374</xdr:colOff>
-      <xdr:row>579</xdr:row>
-      <xdr:rowOff>63406</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>551948</xdr:colOff>
-      <xdr:row>595</xdr:row>
-      <xdr:rowOff>151914</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="135" name="Picture 134">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80A6AF04-FF0F-4369-8361-5F8AEDBE1750}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11987249" y="113791906"/>
-          <a:ext cx="4304762" cy="3136508"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>380368</xdr:colOff>
-      <xdr:row>579</xdr:row>
-      <xdr:rowOff>22906</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>328979</xdr:colOff>
-      <xdr:row>595</xdr:row>
-      <xdr:rowOff>111414</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="136" name="Picture 135">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E14999AD-CFF9-4AF1-AC38-B81D006AD6A9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6595431" y="113751406"/>
-          <a:ext cx="4711111" cy="3136508"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>598</xdr:row>
-      <xdr:rowOff>120950</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>75595</xdr:colOff>
-      <xdr:row>615</xdr:row>
-      <xdr:rowOff>18958</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="137" name="Picture 136">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C001D12B-2910-4C73-B3DB-A520E0823A41}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="857250" y="117468950"/>
-          <a:ext cx="4838095" cy="3136508"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>559141</xdr:colOff>
-      <xdr:row>599</xdr:row>
-      <xdr:rowOff>167042</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>152196</xdr:colOff>
-      <xdr:row>616</xdr:row>
-      <xdr:rowOff>65050</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="138" name="Picture 137">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CF5E2E7-267F-4389-8E74-17F184F88707}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6774204" y="117705542"/>
-          <a:ext cx="4355555" cy="3136508"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>107334</xdr:colOff>
-      <xdr:row>600</xdr:row>
-      <xdr:rowOff>74587</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>67131</xdr:colOff>
-      <xdr:row>616</xdr:row>
-      <xdr:rowOff>163095</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="139" name="Picture 138">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35FA55F2-215F-403C-9B53-8BFA8D3F8889}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12275522" y="117803587"/>
-          <a:ext cx="4126984" cy="3136508"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -20617,7 +20067,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -20667,7 +20117,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -20717,7 +20167,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId52">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -20732,6 +20182,656 @@
         <a:xfrm>
           <a:off x="6647113" y="126157092"/>
           <a:ext cx="7772400" cy="4468143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>555</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>117021</xdr:colOff>
+      <xdr:row>574</xdr:row>
+      <xdr:rowOff>188026</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="58" name="Picture 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C520E821-F7B0-4907-822C-540F06908E08}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="857250" y="109156500"/>
+          <a:ext cx="6613071" cy="3807526"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>267948</xdr:colOff>
+      <xdr:row>534</xdr:row>
+      <xdr:rowOff>162570</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>552150</xdr:colOff>
+      <xdr:row>551</xdr:row>
+      <xdr:rowOff>60578</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="59" name="Picture 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5B281C3-4141-429E-9DCA-C5A0A40FE225}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5824198" y="105318570"/>
+          <a:ext cx="3221077" cy="3136508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>4062</xdr:colOff>
+      <xdr:row>515</xdr:row>
+      <xdr:rowOff>60219</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>524325</xdr:colOff>
+      <xdr:row>533</xdr:row>
+      <xdr:rowOff>148727</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="60" name="Picture 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FF387A1-D535-4221-A507-69E5018EC19B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10259312" y="101596719"/>
+          <a:ext cx="3457138" cy="3517508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>279116</xdr:colOff>
+      <xdr:row>534</xdr:row>
+      <xdr:rowOff>97971</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>235888</xdr:colOff>
+      <xdr:row>550</xdr:row>
+      <xdr:rowOff>186479</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="61" name="Picture 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF9FF27D-3688-4213-B911-CB886ADD6E3A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10534366" y="105253971"/>
+          <a:ext cx="2893647" cy="3136508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>534</xdr:row>
+      <xdr:rowOff>46982</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>18543</xdr:colOff>
+      <xdr:row>550</xdr:row>
+      <xdr:rowOff>135490</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="63" name="Picture 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{655D557A-AB4D-4A1E-A5CB-8F988402868D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="920750" y="105202982"/>
+          <a:ext cx="4066668" cy="3136508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>238786</xdr:colOff>
+      <xdr:row>598</xdr:row>
+      <xdr:rowOff>128853</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>337806</xdr:colOff>
+      <xdr:row>615</xdr:row>
+      <xdr:rowOff>26861</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="65" name="Picture 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE6C5E33-EB7A-4086-A35C-D18854A70849}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6382411" y="117476853"/>
+          <a:ext cx="4210645" cy="3136508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>411155</xdr:colOff>
+      <xdr:row>580</xdr:row>
+      <xdr:rowOff>115566</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>359766</xdr:colOff>
+      <xdr:row>597</xdr:row>
+      <xdr:rowOff>13574</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="66" name="Picture 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9D61B24-745C-4F36-94A2-B2D84BC33B3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11253780" y="114034566"/>
+          <a:ext cx="4647611" cy="3136508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>163068</xdr:colOff>
+      <xdr:row>598</xdr:row>
+      <xdr:rowOff>167247</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>122865</xdr:colOff>
+      <xdr:row>615</xdr:row>
+      <xdr:rowOff>65255</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="67" name="Picture 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3ECFA19D-F1B1-4897-B9BD-D72BA70A1F8A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11593068" y="117515247"/>
+          <a:ext cx="4071422" cy="3136508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>398499</xdr:colOff>
+      <xdr:row>580</xdr:row>
+      <xdr:rowOff>38553</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>527613</xdr:colOff>
+      <xdr:row>596</xdr:row>
+      <xdr:rowOff>127061</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="68" name="Picture 67">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB4CB37C-BC7A-4662-9FF3-C9ED4671BABF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5954749" y="113957553"/>
+          <a:ext cx="4828114" cy="3136508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>535858</xdr:colOff>
+      <xdr:row>580</xdr:row>
+      <xdr:rowOff>39839</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>208288</xdr:colOff>
+      <xdr:row>596</xdr:row>
+      <xdr:rowOff>128347</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="70" name="Picture 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBCFDA6B-0EA5-4383-87A0-22DFB89256E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="805733" y="113958839"/>
+          <a:ext cx="4371430" cy="3136508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>111125</xdr:colOff>
+      <xdr:row>515</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2748</xdr:colOff>
+      <xdr:row>531</xdr:row>
+      <xdr:rowOff>88508</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F79582FC-08C3-F460-CD67-F10B24C80D84}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="968375" y="101536500"/>
+          <a:ext cx="3415873" cy="3136508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>515</xdr:row>
+      <xdr:rowOff>174625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>510788</xdr:colOff>
+      <xdr:row>532</xdr:row>
+      <xdr:rowOff>72633</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF8CC048-A092-5C66-2BC1-F549D96EBBD2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId52">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5905500" y="101711125"/>
+          <a:ext cx="3098413" cy="3136508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>599</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>139095</xdr:colOff>
+      <xdr:row>615</xdr:row>
+      <xdr:rowOff>88508</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E189D074-460D-B408-1D9C-F1DB21763580}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="857250" y="117538500"/>
+          <a:ext cx="4838095" cy="3136508"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -21008,7 +21108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B13:L41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
@@ -22146,8 +22246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:S482"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T482" sqref="T482"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A382" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AE415" sqref="AE415"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -22603,8 +22703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B1:S679"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A667" sqref="A667:XFD667"/>
+    <sheetView showGridLines="0" topLeftCell="A548" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AG599" sqref="AG599"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>

</xml_diff>